<commit_message>
version 0.1 digitalWrite/digitalRead/analogWrite/analogRead pb test analogRead (test ne va pas au bout et se relance en boucle)
</commit_message>
<xml_diff>
--- a/Courses.xlsx
+++ b/Courses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\ProjetElectroPerso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\RepoGit\MyArduinoProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="123">
   <si>
     <t>*** Cette feuille doit rester masquée ***</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>http://fr.aliexpress.com/item/IIC-I2C-Logic-Level-Converter-Bi-Directional-Module-5V-to-3-3V-For-Arduino/32589088559.html</t>
+  </si>
+  <si>
+    <t>recu le 01/07/2016</t>
   </si>
 </sst>
 </file>
@@ -2538,8 +2541,8 @@
   </sheetPr>
   <dimension ref="B1:M61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" customHeight="1"/>
@@ -4326,7 +4329,9 @@
         <f>IFERROR(Liste[QTÉ]*Liste[PRIX UNITAIRE],"")</f>
         <v>0.98</v>
       </c>
-      <c r="K60" s="11"/>
+      <c r="K60" s="11" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="61" spans="3:11" ht="21" customHeight="1">
       <c r="C61" s="20" t="str">
@@ -4352,7 +4357,9 @@
         <f>IFERROR(Liste[QTÉ]*Liste[PRIX UNITAIRE],"")</f>
         <v>0.44</v>
       </c>
-      <c r="K61" s="11"/>
+      <c r="K61" s="11" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10:K10 C8:C9 C12:K16 C11 E11:K11 C17 C20:C21 E20:K21 E17:K17 E8:K9 C22:K22 C6:K7 C5:J5 C18:K19">

</xml_diff>